<commit_message>
Add backlog and use cases test
</commit_message>
<xml_diff>
--- a/PREGAME/1. ELICITACIÓN/1.3 Historias de Usuario/Matriz_Marco_Trabajo_HU_G#5_V1.xlsx
+++ b/PREGAME/1. ELICITACIÓN/1.3 Historias de Usuario/Matriz_Marco_Trabajo_HU_G#5_V1.xlsx
@@ -6,18 +6,20 @@
     <sheet state="visible" name="Formato descripción HU" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Historia de Usuario" sheetId="2" r:id="rId5"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Formato descripción HU'!$B$5:$O$17</definedName>
+  </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="5h3HIVUZCHZTxaIoCNgi5wiZgNiPUgiIchV5r32zP9s="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="YMD3hvMVxTUkkgFi4y4xiYnB5UlEiF06pOtge+bFdwI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="131">
   <si>
     <t>Matriz de Marco de Trabajo de HU</t>
   </si>
@@ -68,7 +70,7 @@
     <t xml:space="preserve">NOMBRE DE HISTORIA </t>
   </si>
   <si>
-    <t>REQ001</t>
+    <t>HU001</t>
   </si>
   <si>
     <t>El aplicativo debe permitir seleccionar un periodo académico para la elaboración de la matriz de carga horaria</t>
@@ -89,43 +91,52 @@
     <t>Kevin Chuquimarca</t>
   </si>
   <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Terminado</t>
+  </si>
+  <si>
+    <t>Mostrar: Periodo académico seleccionado / No se pueden realizar cambios sobre este periodo académico</t>
+  </si>
+  <si>
+    <t>La información del periodo académico se presentara en un campo de la interfaz de elaboración de la matriz de carga horaria</t>
+  </si>
+  <si>
+    <t>Selección de Periodo Académico</t>
+  </si>
+  <si>
+    <t>HU002</t>
+  </si>
+  <si>
+    <t>El aplicativo debe permitir el registro del horario de trabajo de los docentes para la matriz de carga horaria.</t>
+  </si>
+  <si>
+    <t>Registrar el horario de trabajo</t>
+  </si>
+  <si>
+    <t>Para el registro de la hora de entrada y salida para cada día de la semana</t>
+  </si>
+  <si>
+    <t>En el formulario para el registro del horario de trabajo, se debe ingresar la hora para el día, la jornada, si es ingreso o salida, la modalidad físico o virtual.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Media </t>
   </si>
   <si>
     <t>En proceso</t>
   </si>
   <si>
-    <t>Mostrar: Periodo académico seleccionado / No se pueden realizar cambios sobre este periodo académico</t>
-  </si>
-  <si>
-    <t>La información del periodo académico se presentara en un campo de la interfaz de elaboración de la matriz de carga horaria</t>
-  </si>
-  <si>
-    <t>Selección de Periodo Académico</t>
-  </si>
-  <si>
-    <t>REQ002</t>
-  </si>
-  <si>
-    <t>El aplicativo debe permitir el registro del horario de trabajo de los docentes para la matriz de carga horaria.</t>
-  </si>
-  <si>
-    <t>Registrar el horario de trabajo</t>
-  </si>
-  <si>
-    <t>Para el registro de la hora de entrada y salida para cada día de la semana</t>
-  </si>
-  <si>
-    <t>En el formulario para el registro del horario de trabajo, se debe ingresar la hora para el día, la jornada, si es ingreso o salida, la modalidad físico o virtual.</t>
-  </si>
-  <si>
     <t>Información guardada con éxito, en la vista previa de la matriz de carga horaria, se muestra el horario de trabajo registrado.</t>
   </si>
   <si>
+    <t>La información del horario de trabajo se encuentra dispuesta sobre la plantilla en formato PDF para su vista preliminar.</t>
+  </si>
+  <si>
     <t>Registrar horario de trabajo</t>
   </si>
   <si>
-    <t>REQ003</t>
+    <t>HU003</t>
   </si>
   <si>
     <t>El aplicativo debe permitir el registro del horario de clase, especificando cada materia, horas y aulas.</t>
@@ -149,13 +160,16 @@
     <t>Información guardada con éxito, en la vista previa de la matriz de carga horaria, se muestra el horario de clase registrado.</t>
   </si>
   <si>
+    <t>La información del horario de clases se encuentra dispuesta sobre la plantilla en formato PDF para su vista preliminar.</t>
+  </si>
+  <si>
     <t>Registrar horario de clase</t>
   </si>
   <si>
-    <t>REQ004</t>
-  </si>
-  <si>
-    <t>El aplicativo debe controlar que las actividades que son obligatorias para los docentes se registren en la matriz de carga horaria.</t>
+    <t>HU004</t>
+  </si>
+  <si>
+    <t>El aplicativo debe controlar que las actividades que son obligatorias para los docentes se agreguen en la matriz de carga horaria.</t>
   </si>
   <si>
     <t>Control de actividades obligatorias</t>
@@ -164,13 +178,19 @@
     <t>Para controlar que las actividades obligatorias de cada docente se incluyan en la matriz de carga horaria</t>
   </si>
   <si>
-    <t>Durante el registro de actividades, el sistema debe controlar que las actividades que son obligatorias se incluyan en la matriz de carga horaria.</t>
+    <t>Durante la selección del periodo academico para la matriz, el sistema debe controlar que las actividades que son obligatorias se incluyan en la matriz de carga horaria.</t>
+  </si>
+  <si>
+    <t>El listado de actividades obligatorias debe relacionarse con la matriz de carga horaria que se crea al escoger el periodo académico</t>
+  </si>
+  <si>
+    <t>La información de las actividades obligatorias se encuentra dispuesta sobre la plantilla en formato PDF para su vista preliminar</t>
   </si>
   <si>
     <t>Actividades obligatorias</t>
   </si>
   <si>
-    <t>REQ005</t>
+    <t>HU005</t>
   </si>
   <si>
     <t>El aplicativo debe permitir seleccionar las actividades de docencia, Investigación, gestión educativa y vinculación con la sociedad.</t>
@@ -190,10 +210,13 @@
 - vinculación con la sociedad</t>
   </si>
   <si>
+    <t>La información de las actividades registradas por el docente se encuentra dispuesta sobre la plantilla en formato PDF para su vista preliminar</t>
+  </si>
+  <si>
     <t>Registro de actividades</t>
   </si>
   <si>
-    <t>REQ006</t>
+    <t>HU006</t>
   </si>
   <si>
     <t>El aplicativo debe controlar y validar que las actividades seleccionadas por los docentes no sobrepasen las horas que debe cumplir cada tipo de docente.</t>
@@ -208,172 +231,175 @@
     <t xml:space="preserve">Se debe llevar un conteo de las horas por actividad que va seleccionando el docente, y controlar que la suma de las horas de las actividades seleccionadas no sobrepasen las horas que debe cumplir el docente, segun el tipo de contrato que tenga. </t>
   </si>
   <si>
+    <t>La información del horario de clases se encuentran dispuesta sobre la plantilla en formato pdf para su vista preliminar</t>
+  </si>
+  <si>
     <t>Validación de las actividades</t>
   </si>
   <si>
+    <t>HU007</t>
+  </si>
+  <si>
+    <t>El aplicativo debe generar el documento de matriz de carga horaria a partir de la información registrada para el periodo académico seleccionado</t>
+  </si>
+  <si>
+    <t>Generar la matriz de carga horaria</t>
+  </si>
+  <si>
+    <t>Para la generación del documento de la matriz de carga horaria docente</t>
+  </si>
+  <si>
+    <t>Una vez se haya terminado con el registro de la matriz de carga horaria, el aplicativo debe permitir generar un archivo pdf para una vista previa</t>
+  </si>
+  <si>
+    <t>Kevin Chuquimarca - Marco Iza</t>
+  </si>
+  <si>
+    <t>Mostrar: Información guardada con éxito/ Se deben completar los campos obligatorios</t>
+  </si>
+  <si>
+    <t>Se debe habilitar la opción para la vista preliminar del documento en formato pdf con la información ingresada en el aplicativo</t>
+  </si>
+  <si>
+    <t>Generación de matriz</t>
+  </si>
+  <si>
+    <t>HU008</t>
+  </si>
+  <si>
+    <t>El aplicativo debe permitir el envio de la matriz de carga horaria generada para su revisión y aprobación</t>
+  </si>
+  <si>
+    <t>Enviar la matriz de carga horaria para su revisión</t>
+  </si>
+  <si>
+    <t>Para la revisión y respectiva aprobación u observaciones en caso de ser necesario</t>
+  </si>
+  <si>
+    <t>En la interfaz de vista preliminar seleccionar la opción para enviar y posteriormente confirmar la acción</t>
+  </si>
+  <si>
+    <t>Mostrar: Documento enviado para revisión</t>
+  </si>
+  <si>
+    <t>Se debe cambiar el status del documento mostrando en la interfaz de vista preliminar del documento el cambio</t>
+  </si>
+  <si>
+    <t>Envío de matriz</t>
+  </si>
+  <si>
+    <t>HU009</t>
+  </si>
+  <si>
+    <t>El aplicativo debe permitir visualizar los documentos enviados para su revisión y aprobación.</t>
+  </si>
+  <si>
+    <t>Mostrar las matrices de carga horaria</t>
+  </si>
+  <si>
+    <t>Para la visualización estructurada de la información de las matrices de carga horaria enviadas por los docentes</t>
+  </si>
+  <si>
+    <t>Coordinador docente</t>
+  </si>
+  <si>
+    <t>Acceder con el rol de Coordinador de Docencia: De la lista de matrices seleccionar el ícono con un ojo para acceder a la información</t>
+  </si>
+  <si>
+    <t>Mostrar: Cargando matriz de carga horaria para revisión</t>
+  </si>
+  <si>
+    <t>Se presenta el documento en formato pdf en la interfaz de revisión del coordinador docente.</t>
+  </si>
+  <si>
+    <t>Visualización Matrices de Carga Horaria</t>
+  </si>
+  <si>
+    <t>HU010</t>
+  </si>
+  <si>
+    <t>El aplicativo debe permitirles al coordinador de docencia realizar modificaciones de la información de la matriz de carga horaria de los docentes</t>
+  </si>
+  <si>
+    <t>Modificación de matrices de carga horaria Coordinación de Docencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para la modificación de cambios rápidos necesarios para la aprobación de las matrices de carga horaria </t>
+  </si>
+  <si>
+    <t>Coordinador de docencia</t>
+  </si>
+  <si>
+    <t>Seleccionar la opción de realizar cambios para acceder a la interfaz de edición de la información</t>
+  </si>
+  <si>
+    <t>Mostrar: Modo de edición</t>
+  </si>
+  <si>
+    <t>Se cambia el status del documento a revisado y corregido. Se genera un nuevo documento con la información actualizada.</t>
+  </si>
+  <si>
+    <t>Edición de matriz de carga horaria de Coordinación de Docencia</t>
+  </si>
+  <si>
+    <t>HU011</t>
+  </si>
+  <si>
+    <t>El aplicativo debe permitirle al coordinador de docencia realizar observaciones en caso de requerirlo</t>
+  </si>
+  <si>
+    <t>Observaciones sobre matrices de carga horaria</t>
+  </si>
+  <si>
+    <t>Para la realización de observaciones sobre cambios que requieran mayor atención por parte del docente</t>
+  </si>
+  <si>
+    <t>Seleccionar la opción de realizar observaciones sobre el documento actual</t>
+  </si>
+  <si>
+    <t>Mostrar: Observaciones realizadas sobre el documento</t>
+  </si>
+  <si>
+    <t>Se cambia el status del documento a revisado y rechazado. Se envía la observación al propietario del documento.</t>
+  </si>
+  <si>
+    <t>HU012</t>
+  </si>
+  <si>
+    <t>El aplicativo debe permitirle a los docentes realizar modificaciones de la información de la matriz de carga horaria</t>
+  </si>
+  <si>
+    <t>Modificación de matrices de carga horaria Docentes</t>
+  </si>
+  <si>
+    <t>Para la modificación de la información en base a las observaciones realizadas por Coordinación de Docencia</t>
+  </si>
+  <si>
+    <t>Henry Tiamba</t>
+  </si>
+  <si>
+    <t>Mostrar: Tiene cambios por realizar</t>
+  </si>
+  <si>
+    <t>Se habilita el envío del documento para nuevamente ser revisado. Se genera un nuevo documento con la información actualizada.</t>
+  </si>
+  <si>
+    <t>Edición de matriz de carga horaria de Docentes</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>Atrasado</t>
+  </si>
+  <si>
+    <t>HISTORIA DE USUARIO (HU)</t>
+  </si>
+  <si>
+    <t>USUARIO</t>
+  </si>
+  <si>
     <t>REQ007</t>
-  </si>
-  <si>
-    <t>El aplicativo debe generar el documento de matriz de carga horaria a partir de la información registrada para el periodo académico seleccionado</t>
-  </si>
-  <si>
-    <t>Generar la matriz de carga horaria</t>
-  </si>
-  <si>
-    <t>Para la generación del documento de la matriz de carga horaria docente</t>
-  </si>
-  <si>
-    <t>Una vez se haya terminado con el registro de la matriz de carga horaria, el aplicativo debe permitir generar un archivo pdf para una vista previa</t>
-  </si>
-  <si>
-    <t>Kevin Chuquimarca - Marco Iza</t>
-  </si>
-  <si>
-    <t>Alta</t>
-  </si>
-  <si>
-    <t>Mostrar: Información guardada con éxito/ Se deben completar los campos obligatorios</t>
-  </si>
-  <si>
-    <t>Se debe habilitar la opción para la vista preliminar del documento en formato pdf con la información ingresada en el aplicativo</t>
-  </si>
-  <si>
-    <t>Elaboración de matriz</t>
-  </si>
-  <si>
-    <t>REQ008</t>
-  </si>
-  <si>
-    <t>El aplicativo debe permitir el envio de la matriz de carga horaria generada para su revisión y aprobación</t>
-  </si>
-  <si>
-    <t>Enviar la matriz de carga horaria para su revisión</t>
-  </si>
-  <si>
-    <t>Para la revisión y respectiva aprobación u observaciones en caso de ser necesario</t>
-  </si>
-  <si>
-    <t>En la interfaz de vista preliminar seleccionar la opción para enviar y posteriomente confirmar la acción</t>
-  </si>
-  <si>
-    <t>Mostrar: Documento enviado para revisión</t>
-  </si>
-  <si>
-    <t>Se debe cambiar el status del documento mostrando en la interfaz de vista preliminar del documento el cambio</t>
-  </si>
-  <si>
-    <t>Envío de matriz</t>
-  </si>
-  <si>
-    <t>REQ009</t>
-  </si>
-  <si>
-    <t>El aplicativo debe permitir visualizar los documentos enviados para su revisión y aprobación.</t>
-  </si>
-  <si>
-    <t>Mostrar las matrices de carga horaria</t>
-  </si>
-  <si>
-    <t>Para la visualización estructurada de la información de las matrices de carga horaria enviadas por los docentes</t>
-  </si>
-  <si>
-    <t>Coordinador docente</t>
-  </si>
-  <si>
-    <t>Acceder con el rol de Coordinador de Docencia: De la lista de matrices seleccionar el ícono con un ojo para acceder a la información</t>
-  </si>
-  <si>
-    <t>Mostrar: Cargando matriz de carga horaria para revisión</t>
-  </si>
-  <si>
-    <t>Se presenta el documento en formato pdf en la interfaz de revisión del coordinador docente.</t>
-  </si>
-  <si>
-    <t>Matrices de Carga Horaria</t>
-  </si>
-  <si>
-    <t>REQ010</t>
-  </si>
-  <si>
-    <t>El aplicativo debe permitirles al coordinador de docencia realizar modificaciones de la información de la matriz de carga horaria de los docentes</t>
-  </si>
-  <si>
-    <t>Modificación de matrices de carga horaria Coordinación de Docencia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Para la modificación de cambios rápidos necesarios para la aprobación de las matrices de carga horaria </t>
-  </si>
-  <si>
-    <t>Seleccionar la opción de realizar cambios para acceder a la interfaz de edición de la información</t>
-  </si>
-  <si>
-    <t>Mostrar: Modo de edición</t>
-  </si>
-  <si>
-    <t>Se cambia el status del documento a revisado y corregido. Se genera un nuevo documento con la información actualizada.</t>
-  </si>
-  <si>
-    <t>Edición de matriz de carga horaria de Coordinación de Docencia</t>
-  </si>
-  <si>
-    <t>REQ011</t>
-  </si>
-  <si>
-    <t>El aplicativo debe permitirle al coordinador de docencia realizar observaciones en caso de requerirlo</t>
-  </si>
-  <si>
-    <t>Observaciones sobre matrices de carga horaria</t>
-  </si>
-  <si>
-    <t>Para la realización de observaciones sobre cambios que requieran mayor atención por parte del docente</t>
-  </si>
-  <si>
-    <t>Seleccionar la opción de realizar observaciones sobre el documento actual</t>
-  </si>
-  <si>
-    <t>Mostrar: Observaciones realizadas sobre el documento</t>
-  </si>
-  <si>
-    <t>Se cambia el status del documento a revisado y rechazado. Se envía la observación al propietario del documento.</t>
-  </si>
-  <si>
-    <t>REQ012</t>
-  </si>
-  <si>
-    <t>El aplicativo debe permitirle a los docentes realizar modificaciones de la información de la matriz de carga horaria</t>
-  </si>
-  <si>
-    <t>Modificación de matrices de carga horaria Docentes</t>
-  </si>
-  <si>
-    <t>Para la modificación de la información en base a las observaciones realizadas por Coordinación de Docencia</t>
-  </si>
-  <si>
-    <t>Henry Tiamba</t>
-  </si>
-  <si>
-    <t>Mostrar: Tiene cambios por realizar</t>
-  </si>
-  <si>
-    <t>Se habilita el envío del documento para nuevamente ser revisado. Se genera un nuevo documento con la información actualizada.</t>
-  </si>
-  <si>
-    <t>Edición de matriz de carga horaria de Docentes</t>
-  </si>
-  <si>
-    <t>Baja</t>
-  </si>
-  <si>
-    <t>Terminado</t>
-  </si>
-  <si>
-    <t>Atrasado</t>
-  </si>
-  <si>
-    <t>HISTORIA DE USUARIO (HU)</t>
-  </si>
-  <si>
-    <t>USUARIO</t>
   </si>
   <si>
     <t>TIEMPO</t>
@@ -826,7 +852,7 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1001,7 +1027,7 @@
     <xdr:ext cx="1066800" cy="1162050"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1029,7 +1055,7 @@
     <xdr:ext cx="1095375" cy="1162050"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1406,40 +1432,42 @@
         <v>45300.0</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" ht="102.75" customHeight="1">
       <c r="B8" s="8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I8" s="10">
         <v>10.0</v>
@@ -1448,40 +1476,42 @@
         <v>45303.0</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" s="13" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="9" ht="94.5" customHeight="1">
       <c r="B9" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I9" s="10">
         <v>6.0</v>
@@ -1490,35 +1520,39 @@
         <v>45305.0</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="M9" s="14"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" ht="179.25" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>21</v>
@@ -1530,35 +1564,39 @@
         <v>45305.0</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="M10" s="14"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9" t="s">
-        <v>54</v>
+        <v>43</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10" s="13" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11" ht="142.5" customHeight="1">
       <c r="B11" s="8" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>21</v>
@@ -1570,38 +1608,40 @@
         <v>45305.0</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M11" s="14"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9" t="s">
-        <v>60</v>
+      <c r="N11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="O11" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="12" ht="102.0" customHeight="1">
       <c r="B12" s="8" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="I12" s="15">
         <v>12.0</v>
@@ -1610,42 +1650,42 @@
         <v>45294.0</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>70</v>
+        <v>76</v>
+      </c>
+      <c r="O12" s="13" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="13" ht="72.0" customHeight="1">
       <c r="B13" s="8" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I13" s="15">
         <v>16.0</v>
@@ -1654,40 +1694,40 @@
         <v>45299.0</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="O13" s="9" t="s">
-        <v>78</v>
+        <v>84</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="P13" s="17"/>
     </row>
     <row r="14" ht="90.0" customHeight="1">
       <c r="B14" s="8" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>21</v>
@@ -1699,42 +1739,42 @@
         <v>45306.0</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="O14" s="10" t="s">
-        <v>87</v>
+        <v>93</v>
+      </c>
+      <c r="O14" s="13" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="15" ht="103.5" customHeight="1">
       <c r="B15" s="8" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I15" s="10">
         <v>10.0</v>
@@ -1743,39 +1783,39 @@
         <v>45313.0</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="O15" s="10" t="s">
-        <v>95</v>
+        <v>102</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="16" ht="84.75" customHeight="1">
       <c r="B16" s="8" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>21</v>
@@ -1787,42 +1827,42 @@
         <v>45320.0</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="O16" s="10" t="s">
-        <v>98</v>
+        <v>110</v>
+      </c>
+      <c r="O16" s="13" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="17" ht="87.75" customHeight="1">
       <c r="B17" s="8" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="I17" s="15">
         <v>6.0</v>
@@ -1831,19 +1871,19 @@
         <v>45320.0</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="O17" s="10" t="s">
-        <v>110</v>
+        <v>117</v>
+      </c>
+      <c r="O17" s="13" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="18" ht="68.25" customHeight="1">
@@ -1880,10 +1920,10 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="2" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M23" s="5"/>
     </row>
@@ -1891,10 +1931,10 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="M24" s="5"/>
     </row>
@@ -1902,10 +1942,10 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
       <c r="M25" s="5"/>
     </row>
@@ -1914,7 +1954,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="2"/>
       <c r="L26" s="1" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="M26" s="5"/>
     </row>
@@ -7741,6 +7781,7 @@
     <row r="1007" ht="15.75" customHeight="1"/>
     <row r="1008" ht="15.75" customHeight="1"/>
   </sheetData>
+  <autoFilter ref="$B$5:$O$17"/>
   <mergeCells count="1">
     <mergeCell ref="B3:O3"/>
   </mergeCells>
@@ -7792,7 +7833,7 @@
     </row>
     <row r="6" ht="39.75" customHeight="1">
       <c r="B6" s="21" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
@@ -7848,7 +7889,7 @@
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="33" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="32"/>
@@ -7867,18 +7908,18 @@
     <row r="10" ht="30.0" customHeight="1">
       <c r="B10" s="30"/>
       <c r="C10" s="36" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="38" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O17,5,0)</f>
-        <v>Docente</v>
+        <v>#N/A</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="39"/>
       <c r="H10" s="38" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O17,11,0)</f>
-        <v>No iniciado</v>
+        <v>#N/A</v>
       </c>
       <c r="I10" s="23"/>
       <c r="J10" s="39"/>
@@ -7909,7 +7950,7 @@
     <row r="12" ht="30.0" customHeight="1">
       <c r="B12" s="30"/>
       <c r="C12" s="31" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="33" t="s">
@@ -7918,7 +7959,7 @@
       <c r="F12" s="23"/>
       <c r="G12" s="39"/>
       <c r="H12" s="33" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="I12" s="23"/>
       <c r="J12" s="39"/>
@@ -7931,20 +7972,20 @@
     </row>
     <row r="13" ht="30.0" customHeight="1">
       <c r="B13" s="30"/>
-      <c r="C13" s="42">
+      <c r="C13" s="42" t="str">
         <f>VLOOKUP('Historia de Usuario'!C10,'Formato descripción HU'!B6:O17,8,0)</f>
-        <v>12</v>
+        <v>#N/A</v>
       </c>
       <c r="D13" s="37"/>
       <c r="E13" s="38" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O17,10,0)</f>
-        <v>Alta</v>
+        <v>#N/A</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="39"/>
       <c r="H13" s="38" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O17,7,0)</f>
-        <v>Kevin Chuquimarca - Marco Iza</v>
+        <v>#N/A</v>
       </c>
       <c r="I13" s="23"/>
       <c r="J13" s="39"/>
@@ -7975,30 +8016,30 @@
     <row r="15" ht="19.5" customHeight="1">
       <c r="B15" s="30"/>
       <c r="C15" s="43" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="D15" s="44" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O17,3,0)</f>
-        <v>Generar la matriz de carga horaria</v>
+        <v>#N/A</v>
       </c>
       <c r="E15" s="45"/>
       <c r="F15" s="34"/>
       <c r="G15" s="43" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="H15" s="44" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O17,4,0)</f>
-        <v>Para la generación del documento de la matriz de carga horaria docente</v>
+        <v>#N/A</v>
       </c>
       <c r="I15" s="46"/>
       <c r="J15" s="45"/>
       <c r="K15" s="34"/>
       <c r="L15" s="43" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="M15" s="44" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O17,6,0)</f>
-        <v>Una vez se haya terminado con el registro de la matriz de carga horaria, el aplicativo debe permitir generar un archivo pdf para una vista previa</v>
+        <v>#N/A</v>
       </c>
       <c r="N15" s="46"/>
       <c r="O15" s="45"/>
@@ -8056,12 +8097,12 @@
     <row r="19" ht="19.5" customHeight="1">
       <c r="B19" s="30"/>
       <c r="C19" s="54" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="D19" s="45"/>
       <c r="E19" s="55" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O17,14,0)</f>
-        <v>Elaboración de matriz</v>
+        <v>#N/A</v>
       </c>
       <c r="F19" s="56"/>
       <c r="G19" s="56"/>
@@ -8112,12 +8153,12 @@
     <row r="22" ht="19.5" customHeight="1">
       <c r="B22" s="30"/>
       <c r="C22" s="61" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D22" s="45"/>
       <c r="E22" s="44" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O17,12,0)</f>
-        <v>Mostrar: Información guardada con éxito/ Se deben completar los campos obligatorios</v>
+        <v>#N/A</v>
       </c>
       <c r="F22" s="46"/>
       <c r="G22" s="46"/>
@@ -8129,7 +8170,7 @@
       <c r="K22" s="45"/>
       <c r="L22" s="44" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O17,13,0)</f>
-        <v>Se debe habilitar la opción para la vista preliminar del documento en formato pdf con la información ingresada en el aplicativo</v>
+        <v>#N/A</v>
       </c>
       <c r="M22" s="46"/>
       <c r="N22" s="46"/>

</xml_diff>